<commit_message>
Spara ny aktivitet och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsredovisning och ganttschema.xlsx
+++ b/dokumentation/Tidsredovisning och ganttschema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60913\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A38240-40D2-4D82-B9FB-57238BCDBB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADBFC3B-EBF7-4D23-9E4F-D3AED39CBE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Uppgift</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Databasmodellering</t>
+  </si>
+  <si>
+    <t>PHP Activities</t>
   </si>
 </sst>
 </file>
@@ -763,8 +766,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C10" totalsRowCount="1">
-  <autoFilter ref="A1:C9" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C12" totalsRowCount="1">
+  <autoFilter ref="A1:C11" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF97FC8A-2932-4FC2-8517-A9F990E92CD6}" name="Datum" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{14DC3050-107A-4381-8655-4E1F0BC3806A}" name="Antal lektioner" totalsRowFunction="sum"/>
@@ -2262,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0DAB7D-AD71-46CF-97AB-9CF7EC5E80ED}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2375,12 +2378,34 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="52">
+        <v>45307</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="52">
+        <v>45309</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <f>SUBTOTAL(109,Tabell2[Antal lektioner])</f>
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hämta enskild aktivitet oh tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsredovisning och ganttschema.xlsx
+++ b/dokumentation/Tidsredovisning och ganttschema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60913\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADBFC3B-EBF7-4D23-9E4F-D3AED39CBE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03F2F83-41A0-4C9D-B563-55354DA77B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Uppgift</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>PHP Activities</t>
+  </si>
+  <si>
+    <t>PHP Spara aktivitet</t>
   </si>
 </sst>
 </file>
@@ -766,8 +769,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C12" totalsRowCount="1">
-  <autoFilter ref="A1:C11" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C13" totalsRowCount="1">
+  <autoFilter ref="A1:C12" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF97FC8A-2932-4FC2-8517-A9F990E92CD6}" name="Datum" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{14DC3050-107A-4381-8655-4E1F0BC3806A}" name="Antal lektioner" totalsRowFunction="sum"/>
@@ -2265,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0DAB7D-AD71-46CF-97AB-9CF7EC5E80ED}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2400,12 +2403,23 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="52">
+        <v>45310</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <f>SUBTOTAL(109,Tabell2[Antal lektioner])</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uppdatera aktivitet och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsredovisning och ganttschema.xlsx
+++ b/dokumentation/Tidsredovisning och ganttschema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60913\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03F2F83-41A0-4C9D-B563-55354DA77B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471891AF-2A3B-4292-A628-3EB900AE9FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Uppgift</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>PHP Spara aktivitet</t>
+  </si>
+  <si>
+    <t>PHP Hämta enskild aktivitet</t>
+  </si>
+  <si>
+    <t>PHP Uppdatera aktivitet</t>
   </si>
 </sst>
 </file>
@@ -769,8 +775,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C13" totalsRowCount="1">
-  <autoFilter ref="A1:C12" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C15" totalsRowCount="1">
+  <autoFilter ref="A1:C14" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF97FC8A-2932-4FC2-8517-A9F990E92CD6}" name="Datum" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{14DC3050-107A-4381-8655-4E1F0BC3806A}" name="Antal lektioner" totalsRowFunction="sum"/>
@@ -2268,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0DAB7D-AD71-46CF-97AB-9CF7EC5E80ED}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2414,12 +2420,34 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="52">
+        <v>45310</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="52">
+        <v>45310</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <f>SUBTOTAL(109,Tabell2[Antal lektioner])</f>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Radera aktivitet och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsredovisning och ganttschema.xlsx
+++ b/dokumentation/Tidsredovisning och ganttschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60913\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471891AF-2A3B-4292-A628-3EB900AE9FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF6C24A-DFE1-4C2B-807C-B5D241F4B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
+    <workbookView xWindow="14316" yWindow="0" windowWidth="8724" windowHeight="12360" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
   </bookViews>
   <sheets>
     <sheet name="Planering" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Uppgift</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Databasmodellering</t>
   </si>
   <si>
-    <t>PHP Activities</t>
-  </si>
-  <si>
     <t>PHP Spara aktivitet</t>
   </si>
   <si>
@@ -169,6 +166,12 @@
   </si>
   <si>
     <t>PHP Uppdatera aktivitet</t>
+  </si>
+  <si>
+    <t>JS Compilation</t>
+  </si>
+  <si>
+    <t>PHP Hämta aktiviteter</t>
   </si>
 </sst>
 </file>
@@ -775,8 +778,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C15" totalsRowCount="1">
-  <autoFilter ref="A1:C14" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C18" totalsRowCount="1">
+  <autoFilter ref="A1:C17" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF97FC8A-2932-4FC2-8517-A9F990E92CD6}" name="Datum" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{14DC3050-107A-4381-8655-4E1F0BC3806A}" name="Antal lektioner" totalsRowFunction="sum"/>
@@ -2274,10 +2277,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0DAB7D-AD71-46CF-97AB-9CF7EC5E80ED}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2391,7 +2394,7 @@
         <v>45307</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
@@ -2399,24 +2402,24 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="52">
-        <v>45309</v>
+        <v>45307</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="52">
-        <v>45310</v>
+        <v>45309</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2424,10 +2427,10 @@
         <v>45310</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2435,19 +2438,52 @@
         <v>45310</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="52">
+        <v>45310</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="52">
+        <v>45313</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="52">
+        <v>45313</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B15">
+      <c r="B18">
         <f>SUBTOTAL(109,Tabell2[Antal lektioner])</f>
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hämta uppgifter sida och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsredovisning och ganttschema.xlsx
+++ b/dokumentation/Tidsredovisning och ganttschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60913\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF6C24A-DFE1-4C2B-807C-B5D241F4B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90E124E-4BCA-4CAB-9667-7375773EBA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14316" yWindow="0" windowWidth="8724" windowHeight="12360" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
+    <workbookView xWindow="8604" yWindow="1008" windowWidth="14436" windowHeight="10608" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
   </bookViews>
   <sheets>
     <sheet name="Planering" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Uppgift</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>PHP Hämta aktiviteter</t>
+  </si>
+  <si>
+    <t>PHP Radera aktivitet</t>
+  </si>
+  <si>
+    <t>PHP Hämta uppgiftssida</t>
   </si>
 </sst>
 </file>
@@ -778,8 +784,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C18" totalsRowCount="1">
-  <autoFilter ref="A1:C17" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C20" totalsRowCount="1">
+  <autoFilter ref="A1:C19" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF97FC8A-2932-4FC2-8517-A9F990E92CD6}" name="Datum" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{14DC3050-107A-4381-8655-4E1F0BC3806A}" name="Antal lektioner" totalsRowFunction="sum"/>
@@ -2277,10 +2283,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0DAB7D-AD71-46CF-97AB-9CF7EC5E80ED}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2478,12 +2484,34 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="52">
+        <v>45314</v>
+      </c>
+      <c r="B18">
+        <v>1.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="52">
+        <v>45314</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <f>SUBTOTAL(109,Tabell2[Antal lektioner])</f>
-        <v>32</v>
+        <v>35.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spara ny post funkar, inga tester klara
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsredovisning och ganttschema.xlsx
+++ b/dokumentation/Tidsredovisning och ganttschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60913\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90E124E-4BCA-4CAB-9667-7375773EBA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5427BF46-6BD7-4EC4-905F-E8ED8487A474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8604" yWindow="1008" windowWidth="14436" windowHeight="10608" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
   </bookViews>
   <sheets>
     <sheet name="Planering" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Uppgift</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>PHP Hämta uppgiftssida</t>
+  </si>
+  <si>
+    <t>PHP Hämta uppgifter datum</t>
   </si>
 </sst>
 </file>
@@ -784,8 +787,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C20" totalsRowCount="1">
-  <autoFilter ref="A1:C19" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C21" totalsRowCount="1">
+  <autoFilter ref="A1:C20" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF97FC8A-2932-4FC2-8517-A9F990E92CD6}" name="Datum" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{14DC3050-107A-4381-8655-4E1F0BC3806A}" name="Antal lektioner" totalsRowFunction="sum"/>
@@ -2283,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0DAB7D-AD71-46CF-97AB-9CF7EC5E80ED}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2506,12 +2509,23 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="52">
+        <v>45315</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <f>SUBTOTAL(109,Tabell2[Antal lektioner])</f>
-        <v>35.5</v>
+        <v>37.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Radera uppgift och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsredovisning och ganttschema.xlsx
+++ b/dokumentation/Tidsredovisning och ganttschema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60913\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F089DAEA-557D-4B64-9B08-E7A4755C9B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42709212-526A-4980-9E42-430BB81F4E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{871BBAF1-ADEF-46A9-88BA-6F0EA735D089}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Uppgift</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>PHP Hämta enskild uppgift + test</t>
+  </si>
+  <si>
+    <t>PHP Uppdatera uppgift</t>
+  </si>
+  <si>
+    <t>PHP Radera uppgift</t>
   </si>
 </sst>
 </file>
@@ -799,8 +805,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C25" totalsRowCount="1">
-  <autoFilter ref="A1:C24" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}" name="Tabell2" displayName="Tabell2" ref="A1:C27" totalsRowCount="1">
+  <autoFilter ref="A1:C26" xr:uid="{F084C4B8-476A-4AD7-840F-23B92CEB5416}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF97FC8A-2932-4FC2-8517-A9F990E92CD6}" name="Datum" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{14DC3050-107A-4381-8655-4E1F0BC3806A}" name="Antal lektioner" totalsRowFunction="sum"/>
@@ -2298,10 +2304,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0DAB7D-AD71-46CF-97AB-9CF7EC5E80ED}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2576,12 +2582,34 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="52">
+        <v>45320</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="52">
+        <v>45320</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <f>SUBTOTAL(109,Tabell2[Antal lektioner])</f>
-        <v>43.5</v>
+        <v>47.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>